<commit_message>
Code clean up und Bugfix for closing and opening same version window again: property change listener now get registered and unregistered properly
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>Story Id</t>
   </si>
@@ -88,6 +88,12 @@
   </si>
   <si>
     <t>Save all versions of one document</t>
+  </si>
+  <si>
+    <t>Erledigt</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -426,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,7 +443,7 @@
     <col min="2" max="2" width="97.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -450,8 +456,11 @@
       <c r="D1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -465,7 +474,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -479,7 +488,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -493,7 +502,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -506,8 +515,11 @@
       <c r="D5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -521,7 +533,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -535,7 +547,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -549,7 +561,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -563,7 +575,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -577,7 +589,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -591,7 +603,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -605,7 +617,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -619,7 +631,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -630,7 +642,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -644,7 +656,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>

</xml_diff>